<commit_message>
se actualizan el archivo donde se tiene el diagrama de Gantt
</commit_message>
<xml_diff>
--- a/Manuales y Documentos/pfcg.xlsx
+++ b/Manuales y Documentos/pfcg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>Manual de Usuario</t>
+  </si>
+  <si>
+    <t>Documento de Requerimentos de Software</t>
   </si>
 </sst>
 </file>
@@ -1312,19 +1315,19 @@
     <xf numFmtId="171" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="170" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - Énfasis1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -1661,7 +1664,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1951,7 +1954,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1965,7 +1968,7 @@
   <dimension ref="A1:CU36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CO1" sqref="CO1:CU1048576"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2045,24 +2048,24 @@
       <c r="B3" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="93"/>
-      <c r="E3" s="91">
+      <c r="D3" s="92"/>
+      <c r="E3" s="95">
         <f>DATE(2021,3,8)</f>
         <v>44263</v>
       </c>
-      <c r="F3" s="91"/>
+      <c r="F3" s="95"/>
     </row>
     <row r="4" spans="1:99" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="93"/>
+      <c r="D4" s="92"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
@@ -2198,12 +2201,12 @@
       <c r="A5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
       <c r="I5" s="81">
         <f>InicioDelProyecto-WEEKDAY(InicioDelProyecto,1)+2+7*(SemanaParaMostrar-1)</f>
         <v>44263</v>
@@ -2856,7 +2859,7 @@
         <v>l</v>
       </c>
       <c r="CB6" s="10" t="str">
-        <f t="shared" ref="CB6:CU6" si="22">LEFT(TEXT(CB5,"ddd"),1)</f>
+        <f t="shared" ref="CB6:CN6" si="22">LEFT(TEXT(CB5,"ddd"),1)</f>
         <v>m</v>
       </c>
       <c r="CC6" s="10" t="str">
@@ -5396,11 +5399,21 @@
     </row>
     <row r="29" spans="1:99" s="3" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="45"/>
-      <c r="B29" s="64"/>
+      <c r="B29" s="87" t="s">
+        <v>59</v>
+      </c>
       <c r="C29" s="60"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="77"/>
+      <c r="D29" s="26">
+        <v>1</v>
+      </c>
+      <c r="E29" s="77">
+        <f>F28</f>
+        <v>44399</v>
+      </c>
+      <c r="F29" s="77">
+        <f>E29+4</f>
+        <v>44403</v>
+      </c>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
       <c r="I29" s="31"/>
@@ -5853,16 +5866,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -5870,6 +5873,16 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="17">

</xml_diff>